<commit_message>
Added affix types for filters
</commit_message>
<xml_diff>
--- a/resources/data-imports/Affixes/accuracy.xlsx
+++ b/resources/data-imports/Affixes/accuracy.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="60">
   <si>
     <t xml:space="preserve">id</t>
   </si>
@@ -137,6 +137,9 @@
   </si>
   <si>
     <t xml:space="preserve">resistance_reduction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">affix_type</t>
   </si>
   <si>
     <t xml:space="preserve">Rangers Eye</t>
@@ -302,10 +305,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AM10"/>
+  <dimension ref="A1:AN10"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K12" activeCellId="0" sqref="K12"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AA1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="AN10" activeCellId="0" sqref="AN10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -458,16 +461,19 @@
       <c r="AM1" s="1" t="s">
         <v>38</v>
       </c>
+      <c r="AN1" s="0" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="n">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="I2" s="1" t="n">
         <v>0.01</v>
@@ -515,7 +521,7 @@
         <v>46</v>
       </c>
       <c r="AA2" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AC2" s="1" t="n">
         <v>0.01</v>
@@ -530,7 +536,7 @@
         <v>1000</v>
       </c>
       <c r="AI2" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="AJ2" s="1" t="n">
         <v>0</v>
@@ -543,6 +549,9 @@
       </c>
       <c r="AM2" s="1" t="n">
         <v>0</v>
+      </c>
+      <c r="AN2" s="0" t="n">
+        <v>7</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -550,10 +559,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="I3" s="1" t="n">
         <v>0.0194</v>
@@ -601,7 +610,7 @@
         <v>91</v>
       </c>
       <c r="AA3" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AC3" s="1" t="n">
         <v>0.0178</v>
@@ -616,7 +625,7 @@
         <v>8918</v>
       </c>
       <c r="AI3" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="AJ3" s="1" t="n">
         <v>0</v>
@@ -629,6 +638,9 @@
       </c>
       <c r="AM3" s="1" t="n">
         <v>0</v>
+      </c>
+      <c r="AN3" s="0" t="n">
+        <v>7</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -636,10 +648,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="I4" s="1" t="n">
         <v>0.0376</v>
@@ -687,7 +699,7 @@
         <v>136</v>
       </c>
       <c r="AA4" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AC4" s="1" t="n">
         <v>0.0316</v>
@@ -702,7 +714,7 @@
         <v>79500</v>
       </c>
       <c r="AI4" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="AJ4" s="1" t="n">
         <v>0</v>
@@ -715,6 +727,9 @@
       </c>
       <c r="AM4" s="1" t="n">
         <v>0</v>
+      </c>
+      <c r="AN4" s="0" t="n">
+        <v>7</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -722,10 +737,10 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="I5" s="1" t="n">
         <v>0.0729</v>
@@ -773,7 +788,7 @@
         <v>181</v>
       </c>
       <c r="AA5" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AC5" s="1" t="n">
         <v>0.0562</v>
@@ -788,7 +803,7 @@
         <v>709200</v>
       </c>
       <c r="AI5" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="AJ5" s="1" t="n">
         <v>0</v>
@@ -801,6 +816,9 @@
       </c>
       <c r="AM5" s="1" t="n">
         <v>0</v>
+      </c>
+      <c r="AN5" s="0" t="n">
+        <v>7</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -808,10 +826,10 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="I6" s="1" t="n">
         <v>0.1414</v>
@@ -859,7 +877,7 @@
         <v>226</v>
       </c>
       <c r="AA6" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AC6" s="1" t="n">
         <v>0.1</v>
@@ -874,7 +892,7 @@
         <v>6324600</v>
       </c>
       <c r="AI6" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="AJ6" s="1" t="n">
         <v>0</v>
@@ -887,6 +905,9 @@
       </c>
       <c r="AM6" s="1" t="n">
         <v>0</v>
+      </c>
+      <c r="AN6" s="0" t="n">
+        <v>7</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -894,10 +915,10 @@
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="I7" s="1" t="n">
         <v>0.2885</v>
@@ -945,7 +966,7 @@
         <v>271</v>
       </c>
       <c r="AA7" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AC7" s="1" t="n">
         <v>0.1871</v>
@@ -960,7 +981,7 @@
         <v>59336800</v>
       </c>
       <c r="AI7" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="AJ7" s="1" t="n">
         <v>0</v>
@@ -973,6 +994,9 @@
       </c>
       <c r="AM7" s="1" t="n">
         <v>0</v>
+      </c>
+      <c r="AN7" s="0" t="n">
+        <v>7</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -980,10 +1004,10 @@
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="I8" s="1" t="n">
         <v>0.5652</v>
@@ -1031,7 +1055,7 @@
         <v>316</v>
       </c>
       <c r="AA8" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AC8" s="1" t="n">
         <v>0.3361</v>
@@ -1046,7 +1070,7 @@
         <v>534551000</v>
       </c>
       <c r="AI8" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="AJ8" s="1" t="n">
         <v>0</v>
@@ -1059,6 +1083,9 @@
       </c>
       <c r="AM8" s="1" t="n">
         <v>0</v>
+      </c>
+      <c r="AN8" s="0" t="n">
+        <v>7</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1066,10 +1093,10 @@
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="I9" s="1" t="n">
         <v>0.88</v>
@@ -1117,7 +1144,7 @@
         <v>361</v>
       </c>
       <c r="AA9" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AC9" s="1" t="n">
         <v>0.6037</v>
@@ -1132,7 +1159,7 @@
         <v>4815640300</v>
       </c>
       <c r="AI9" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="AJ9" s="1" t="n">
         <v>0</v>
@@ -1145,6 +1172,9 @@
       </c>
       <c r="AM9" s="1" t="n">
         <v>0</v>
+      </c>
+      <c r="AN9" s="0" t="n">
+        <v>7</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1152,10 +1182,10 @@
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="I10" s="1" t="n">
         <v>1</v>
@@ -1203,7 +1233,7 @@
         <v>401</v>
       </c>
       <c r="AA10" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AC10" s="1" t="n">
         <v>1</v>
@@ -1218,7 +1248,7 @@
         <v>40000000000</v>
       </c>
       <c r="AI10" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="AJ10" s="1" t="n">
         <v>0</v>
@@ -1231,6 +1261,9 @@
       </c>
       <c r="AM10" s="1" t="n">
         <v>0</v>
+      </c>
+      <c r="AN10" s="0" t="n">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>